<commit_message>
updated categorize notebook, and the generate_answers pipeline
</commit_message>
<xml_diff>
--- a/data/extracted_data/abstracts.xlsx
+++ b/data/extracted_data/abstracts.xlsx
@@ -1127,17 +1127,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>gezmu, andargachew mekonnen (57205400175); nurnberger, andreas (14027288100); bati, tesfaye bayu (56096240400)</t>
+          <t>patel, nitesh g. (57224578760); patel, dhiren b. (57219417636)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>neural machine translation for amharic-english translation</t>
+          <t>nlp-based processing of gujarati compound word sandhis generation and segmentation</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SciTePress</t>
+          <t>Springer</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Gezmu, A. M., et al. “Neural Machine Translation for Amharic-English Translation.” ICAART - Proc. Int. Conf. Agents Artif. Intell., edited by Rocha A.P. et al., vol. 1, SciTePress, 2021, pp. 526–32.</t>
+          <t>Patel, N. G., and D. B. Patel. “NLP-Based Processing of Gujarati Compound Word Sandhi’s Generation and Segmentation.” Lect. Notes Networks Syst., edited by Rathore V.S. et al., vol. 1006 LNNS, Springer Science and Business Media Deutschland GmbH, 2024, pp. 263–71.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1156,47 +1156,43 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>this paper describes neural machine translation between orthographically and morphologically divergent languages. amharic has a rich morphology; it uses the syllabic ethiopic script. we used a new transliteration technique for amharic to facilitate vocabulary sharing. to tackle the highly inflectional morphology and to make an open vocabulary translation, we used subwords. furthermore, the research was conducted on low data conditions. we used the transformer based neural machine translation architecture by tuning the hyperparameters for low data conditions. in the automatic evaluation of the strong baseline, word based, and subword based models trained on a public benchmark dataset, the best subword based models outperform the baseline models by approximately six up to seven bleu. (c) 2021 by scitepress  science and technology publications, lda. all rights reserved</t>
+          <t>in this research paper, we focused on the contribution of rule based "sandhi" splitting and joining methods for the gujarati language, a prominent indian language with a complex linguistic structure. "sandhi" represents a crucial aspect of the language grammar, where words undergo changes when combined, affecting both written and spoken communication. in this study, we explore traditional rule based techniques for splitting and joining gujarati compound words, an integral part of the languages morphology. we examine the effectiveness of these methods in enhancing text processing and comprehension, particularly in the perspective of nlp applications. in this study, we delve into the linguistic intricacies of gujarati sandhi and develop rule based algorithms to effectively split and join words according to established grammatical rules. we explore the application of these methods in various natural language processing tasks, such as text analysis, machine translation, and information retrieval. sandhi splitting (vicched) is a trickier task then sandhi joining for given its ordinariness and context dependency. furthermore, we compare the performance of rule based sandhi methods with other existing approaches, including machine learning based techniques, to evaluate their effectiveness and applicability in different contexts. additionally, we discuss potential enhancements and future directions for incorporating these rule based methods into modern computational linguistics and language processing frameworks. (c) the author(s), under exclusive license to springer nature singapore pte ltd. 2024.</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>low-resource language; neural machine translation; subword</t>
+          <t>gujarati grammar; nlp; rule-based; sandhi; word segmentation; words joining</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>computational linguistics; computer aided language translation; morphology; automatic evaluation; baseline models; benchmark datasets; hyperparameters; machine translations; sub words; artificial intelligence</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>low-resource</t>
-        </is>
-      </c>
+          <t>computational linguistics; joining; learning algorithms; text processing; compound words; gujarati grammar; language processing; research papers; rule based; sandhi; splitting method; splittings; word joining; word segmentation; natural language processing systems</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>morpholog, inflect</t>
+          <t>morpholog</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>amharic (2)</t>
+          <t>gujarati (1)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>amharic (2)</t>
+          <t>gujarati (1)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>amharic (2)</t>
+          <t>gujarati (1)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1212,7 +1208,7 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>Rusty</t>
+          <t>Agustin</t>
         </is>
       </c>
       <c r="V7" t="b">
@@ -1222,7 +1218,7 @@
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>Murilo</t>
+          <t>Ahmad</t>
         </is>
       </c>
       <c r="Z7" t="b">
@@ -1239,17 +1235,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>patel, nitesh g. (57224578760); patel, dhiren b. (57219417636)</t>
+          <t>gezmu, andargachew mekonnen (57205400175); nurnberger, andreas (14027288100); bati, tesfaye bayu (56096240400)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>nlp-based processing of gujarati compound word sandhis generation and segmentation</t>
+          <t>neural machine translation for amharic-english translation</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Springer</t>
+          <t>SciTePress</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1259,7 +1255,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Patel, N. G., and D. B. Patel. “NLP-Based Processing of Gujarati Compound Word Sandhi’s Generation and Segmentation.” Lect. Notes Networks Syst., edited by Rathore V.S. et al., vol. 1006 LNNS, Springer Science and Business Media Deutschland GmbH, 2024, pp. 263–71.</t>
+          <t>Gezmu, A. M., et al. “Neural Machine Translation for Amharic-English Translation.” ICAART - Proc. Int. Conf. Agents Artif. Intell., edited by Rocha A.P. et al., vol. 1, SciTePress, 2021, pp. 526–32.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1268,43 +1264,47 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>in this research paper, we focused on the contribution of rule based "sandhi" splitting and joining methods for the gujarati language, a prominent indian language with a complex linguistic structure. "sandhi" represents a crucial aspect of the language grammar, where words undergo changes when combined, affecting both written and spoken communication. in this study, we explore traditional rule based techniques for splitting and joining gujarati compound words, an integral part of the languages morphology. we examine the effectiveness of these methods in enhancing text processing and comprehension, particularly in the perspective of nlp applications. in this study, we delve into the linguistic intricacies of gujarati sandhi and develop rule based algorithms to effectively split and join words according to established grammatical rules. we explore the application of these methods in various natural language processing tasks, such as text analysis, machine translation, and information retrieval. sandhi splitting (vicched) is a trickier task then sandhi joining for given its ordinariness and context dependency. furthermore, we compare the performance of rule based sandhi methods with other existing approaches, including machine learning based techniques, to evaluate their effectiveness and applicability in different contexts. additionally, we discuss potential enhancements and future directions for incorporating these rule based methods into modern computational linguistics and language processing frameworks. (c) the author(s), under exclusive license to springer nature singapore pte ltd. 2024.</t>
+          <t>this paper describes neural machine translation between orthographically and morphologically divergent languages. amharic has a rich morphology; it uses the syllabic ethiopic script. we used a new transliteration technique for amharic to facilitate vocabulary sharing. to tackle the highly inflectional morphology and to make an open vocabulary translation, we used subwords. furthermore, the research was conducted on low data conditions. we used the transformer based neural machine translation architecture by tuning the hyperparameters for low data conditions. in the automatic evaluation of the strong baseline, word based, and subword based models trained on a public benchmark dataset, the best subword based models outperform the baseline models by approximately six up to seven bleu. (c) 2021 by scitepress  science and technology publications, lda. all rights reserved</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>gujarati grammar; nlp; rule-based; sandhi; word segmentation; words joining</t>
+          <t>low-resource language; neural machine translation; subword</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>computational linguistics; joining; learning algorithms; text processing; compound words; gujarati grammar; language processing; research papers; rule based; sandhi; splitting method; splittings; word joining; word segmentation; natural language processing systems</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
+          <t>computational linguistics; computer aided language translation; morphology; automatic evaluation; baseline models; benchmark datasets; hyperparameters; machine translations; sub words; artificial intelligence</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>low-resource</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>morpholog</t>
+          <t>morpholog, inflect</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>gujarati (1)</t>
+          <t>amharic (2)</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>gujarati (1)</t>
+          <t>amharic (2)</t>
         </is>
       </c>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>gujarati (1)</t>
+          <t>amharic (2)</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1320,7 +1320,7 @@
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr">
         <is>
-          <t>Agustin</t>
+          <t>Rusty</t>
         </is>
       </c>
       <c r="V8" t="b">
@@ -1330,7 +1330,7 @@
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>Ahmad</t>
+          <t>Murilo</t>
         </is>
       </c>
       <c r="Z8" t="b">
@@ -1463,9 +1463,21 @@
           <t>enhancing neural machine translation quality for kannada-tulu language pairs through transformer architecture: a linguistic feature integration</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>International University of Sarajevo</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Supriya, M., et al. “Enhancing Neural Machine Translation Quality for Kannada–Tulu Language Pairs through Transformer Architecture: A Linguistic Feature Integration.” Designs, vol. 8, no. 5, 2024.</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>2024</v>
@@ -18946,7 +18958,11 @@
       <c r="H183" t="n">
         <v>2018</v>
       </c>
-      <c r="I183" t="inlineStr"/>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>quechua is a low-resource language spoken by nearly 9 million persons in south america (hintz and hintz, 2017). yet, in recent times there are few published accounts of successful adaptations of machine translation systems for low-resource languages like quechua. in some cases, machine translations from quechua to spanish are inadequate due to error in alignment. we attempt to improve previous alignment techniques by aligning two languages that are similar due to agglutination: quechua and finnish. our novel technique allows us to add rules that improve alignment for the prediction algorithm used in common machine translation systems.</t>
+        </is>
+      </c>
       <c r="J183" t="inlineStr"/>
       <c r="K183" t="inlineStr"/>
       <c r="L183" t="inlineStr">
@@ -18962,7 +18978,7 @@
       <c r="N183" t="inlineStr"/>
       <c r="O183" t="inlineStr">
         <is>
-          <t>quechua (1), spanish (5)</t>
+          <t>quechua (1), spanish (5), finnish (4)</t>
         </is>
       </c>
       <c r="P183" t="inlineStr">

</xml_diff>